<commit_message>
add successful patch checking
</commit_message>
<xml_diff>
--- a/repair-generation/results/results_introclass.xlsx
+++ b/repair-generation/results/results_introclass.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -467,6 +467,23 @@
         </is>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>median</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>AstorMain-median-3</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>/Users/ruizhengu/Experiments/APR-as-AAT/IntroClassJava/dataset/median/fe9d5fb933c758c2cbbd859e3ecbd2d2eaecc2843b57cfd97da99af24de59f189a144d13ce81ec585d7c2f7367f70c0fb2aec8269eed1fd8380def614817ef7c/002</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
add partial repair results
</commit_message>
<xml_diff>
--- a/repair-generation/results/results_introclass.xlsx
+++ b/repair-generation/results/results_introclass.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -484,6 +484,601 @@
         </is>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>median</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>AstorMain-median-12</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>/Users/ruizhengu/Experiments/APR-as-AAT/IntroClassJava/dataset/median/48b82975576f07f162163145b334648a73321d003a0a8cd4577172e48ce4836e63953dffd4460a9a7aadc511a695ff93de0ce2baf953e4b78b747440caa736a6/000</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>smallest</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>AstorMain-smallest-4</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>/Users/ruizhengu/Experiments/APR-as-AAT/IntroClassJava/dataset/smallest/88394fc00b7053b386e97564e28ef68421ae09c0baeaf887bba7e254f452419783ed8f774bff3c0c7d23bdc8f6c1443fb47c7af97323d4d3d63cc088d3b6841a/006</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>smallest</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>AstorMain-smallest-13</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>/Users/ruizhengu/Experiments/APR-as-AAT/IntroClassJava/dataset/smallest/769cd811312cbbb82c87033a78ac9584ad282550bcb9cc3ae8c4e3da44c288c1a5b3954e01998c3c0654ee6774ceab66e9fe5b135750905c917d2b0bb5fab98b/003</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>smallest</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>AstorMain-smallest-15</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>/Users/ruizhengu/Experiments/APR-as-AAT/IntroClassJava/dataset/smallest/769cd811312cbbb82c87033a78ac9584ad282550bcb9cc3ae8c4e3da44c288c1a5b3954e01998c3c0654ee6774ceab66e9fe5b135750905c917d2b0bb5fab98b/002</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>smallest</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>AstorMain-smallest-27</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>/Users/ruizhengu/Experiments/APR-as-AAT/IntroClassJava/dataset/smallest/3b2376ab97bb5d1a5dbbf2b45cf062db320757549c761936d19df05e856de894e45695014cd8063cdc22148b13fa1803b3c9e77356931d66f4fbec0efacf7829/008</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>smallest</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>AstorMain-smallest-28</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>/Users/ruizhengu/Experiments/APR-as-AAT/IntroClassJava/dataset/smallest/3b2376ab97bb5d1a5dbbf2b45cf062db320757549c761936d19df05e856de894e45695014cd8063cdc22148b13fa1803b3c9e77356931d66f4fbec0efacf7829/006</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>smallest</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>AstorMain-smallest-32</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>/Users/ruizhengu/Experiments/APR-as-AAT/IntroClassJava/dataset/smallest/f8d57deac89e46f99354a70e8f6bc830e0bded0c297d7a0765348de79d6071cb076d4e8f2cd60cff584cb220049d6065827a29904a7e1f9144f510f7773e6d0e/000</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>smallest</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>AstorMain-smallest-35</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>/Users/ruizhengu/Experiments/APR-as-AAT/IntroClassJava/dataset/smallest/dedc2a7c919835ade6d92729cfb18fc71addf6dcdf36ce26ca8b1e3d3aea81bad974c61b96fd71537e95a6aac4582d5b08f9fd8057ce40fb18fb5df37d86b70d/000</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>smallest</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>AstorMain-smallest-40</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>/Users/ruizhengu/Experiments/APR-as-AAT/IntroClassJava/dataset/smallest/95362737dcd262ddd67b0fe1381c25f1e6b885860b4e51efb6f57223dceb77b4c6c7d855e3fe891c10cd51b48c9b052cf2c74f181a28d3020d77a4a2d6e4db18/009</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>smallest</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>AstorMain-smallest-46</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>/Users/ruizhengu/Experiments/APR-as-AAT/IntroClassJava/dataset/smallest/36d8008b13f6475ca8fa4553fea10042b0a6c623665065672051445c3464d61b29b47cb66321844a0264505a0f5ccf5aa6de072aa266b5a8b0cf13198380a389/003</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>smallest</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>AstorMain-smallest-48</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>/Users/ruizhengu/Experiments/APR-as-AAT/IntroClassJava/dataset/smallest/97f6b15278788d90f6a0159ac65668f63f182fadf165e78bfecd7750de89f8611759f8d8206b3505407f7de14d124db7b0309a53e222c538c4dedadc6fa24fe6/003</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>grade</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>AstorMain-grade-1</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>/Users/ruizhengu/Experiments/APR-as-AAT/IntroClassJava/dataset/grade/833bd42c11f7407d63f604b8ba3b7927e22e04e91884c959f01083cda7d5019610705b94a89c09cd1caa3fd1d58eee24b48b85b523db0fa3fc302e7af2dff93d/003</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>grade</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>AstorMain-grade-6</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>/Users/ruizhengu/Experiments/APR-as-AAT/IntroClassJava/dataset/grade/d8b262849e28496f80a8acf7de9758cf3f3a4edf023343521e2e0ac50ec485212a473405570d6c58de6756ae098600d9c7138390faa1aaf6bf3609a8d4016448/000</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>grade</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>AstorMain-grade-8</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>/Users/ruizhengu/Experiments/APR-as-AAT/IntroClassJava/dataset/grade/769cd811312cbbb82c87033a78ac9584ad282550bcb9cc3ae8c4e3da44c288c1a5b3954e01998c3c0654ee6774ceab66e9fe5b135750905c917d2b0bb5fab98b/000</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>grade</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>AstorMain-grade-10</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>/Users/ruizhengu/Experiments/APR-as-AAT/IntroClassJava/dataset/grade/93f87bf20be12abd3b52e14015efb6d78b6038d2022e0ab5889979f9c6b6c8c757d6b5a59feae9f8415158057992ae837da76609dc156ea76b5cca7a43a4678b/015</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>grade</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>AstorMain-grade-20</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>/Users/ruizhengu/Experiments/APR-as-AAT/IntroClassJava/dataset/grade/1c2bb3a40a82cba97b2937bc6825903a28ecfe91f993fc177a0f2ae003bcc7b1073eb49e35d3f0f69d6b612e8347e9c1b93306bf25a7e5390098c1a06845baac/003</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>grade</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>AstorMain-grade-33</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>/Users/ruizhengu/Experiments/APR-as-AAT/IntroClassJava/dataset/grade/d6364e6e98a5c96387950d5b3e6206ba9d57628ab2ad0f2cd05ea7af3b818ed03e514157fe4c64e264a0ac9df0840028e0c5a8fd3d096f5ab93bffba61f23812/007</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>grade</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>AstorMain-grade-36</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>/Users/ruizhengu/Experiments/APR-as-AAT/IntroClassJava/dataset/grade/a0e3fdae706d528dcf146cbad986ba9fd834440a7b500e32f04fad073e955a46e481c713ee118432f3fd5dfa1a63fc1caefd648a56a389e40e6362dfd51625b0/012</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>grade</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>AstorMain-grade-37</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>/Users/ruizhengu/Experiments/APR-as-AAT/IntroClassJava/dataset/grade/a0e3fdae706d528dcf146cbad986ba9fd834440a7b500e32f04fad073e955a46e481c713ee118432f3fd5dfa1a63fc1caefd648a56a389e40e6362dfd51625b0/010</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>grade</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>AstorMain-grade-45</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>/Users/ruizhengu/Experiments/APR-as-AAT/IntroClassJava/dataset/grade/e23b96b6bab26bd14316cefafcbaa16dd8eafcfb97a7159a7772f3c8bb3e78fb353dea728f6b4df6528286af5f0b85fd134c79886c9c2a352fe80d8204c69111/003</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>grade</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>AstorMain-grade-46</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>/Users/ruizhengu/Experiments/APR-as-AAT/IntroClassJava/dataset/grade/e23b96b6bab26bd14316cefafcbaa16dd8eafcfb97a7159a7772f3c8bb3e78fb353dea728f6b4df6528286af5f0b85fd134c79886c9c2a352fe80d8204c69111/004</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>grade</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>AstorMain-grade-55</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>/Users/ruizhengu/Experiments/APR-as-AAT/IntroClassJava/dataset/grade/f5b56c79c624eac7c37c45c1540916bb9b5f5db93e2a426a282a5d0eacde86b4b1e5d1d119eeb06f0ead94d2e4f228dca8dde4ef511af4bc59a18d272d820a0e/010</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>grade</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>AstorMain-grade-56</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>/Users/ruizhengu/Experiments/APR-as-AAT/IntroClassJava/dataset/grade/ee1f20ccded21df47f14019584a29968013d1e66c8df14c1564aff0d69f463c1897e93b7881fa6318cbf475b51e0cdd7523d748525fb5d64d376b88614d3fc92/000</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>grade</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>AstorMain-grade-58</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>/Users/ruizhengu/Experiments/APR-as-AAT/IntroClassJava/dataset/grade/489253253c866aa61b6b0d95c6072d3912f6b78dfbc01bdb2fbb663aefe33d6d353b1a61bb5fc567c9d6c334994111816edd3d43db47e4ea4a84953198736ff7/010</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>grade</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>AstorMain-grade-59</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>/Users/ruizhengu/Experiments/APR-as-AAT/IntroClassJava/dataset/grade/cd2d9b5b5cff96b07c5b22c0d139ffa2aa36b01823c9eb4db6eca19065a0ce2c4d2516bfcc2f1bc95daeae5b0bbd5e9c15b83feda776735e7bc3de6c49d25144/013</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>grade</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>AstorMain-grade-76</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>/Users/ruizhengu/Experiments/APR-as-AAT/IntroClassJava/dataset/grade/dccb1242e60245b164eba39e7c2ae4d7140c2c8964675ee78c7d8bea4aae494217dcac52415ab45fd89391060d17b101d87530b8e5a0b9a5781d06fe7db614eb/001</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>grade</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>AstorMain-grade-77</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>/Users/ruizhengu/Experiments/APR-as-AAT/IntroClassJava/dataset/grade/5b504b3547416bfd54f138b3caa529ad72d157744b787e0e6f4745a2ff0fc5cc33bc87904b2d7cda9c7858087b2e04ece46d53fe9edd208f68d30a0ae70f363f/000</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>grade</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>AstorMain-grade-79</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>/Users/ruizhengu/Experiments/APR-as-AAT/IntroClassJava/dataset/grade/36d8008b13f6475ca8fa4553fea10042b0a6c623665065672051445c3464d61b29b47cb66321844a0264505a0f5ccf5aa6de072aa266b5a8b0cf13198380a389/000</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>grade</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>AstorMain-grade-80</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>/Users/ruizhengu/Experiments/APR-as-AAT/IntroClassJava/dataset/grade/9083480332b4a5e4274f3bf5ef8bd5d1bd75048c0c066e574c27a2de6d919d658efc519e8b6a230a074eb5f2957d5768f4dc981a8e926c3a72993bc448a017f7/013</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>grade</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>AstorMain-grade-82</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>/Users/ruizhengu/Experiments/APR-as-AAT/IntroClassJava/dataset/grade/9083480332b4a5e4274f3bf5ef8bd5d1bd75048c0c066e574c27a2de6d919d658efc519e8b6a230a074eb5f2957d5768f4dc981a8e926c3a72993bc448a017f7/010</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>grade</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>AstorMain-grade-88</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>/Users/ruizhengu/Experiments/APR-as-AAT/IntroClassJava/dataset/grade/cb243bebea400595cc274d1246f3307c507ba6a0e891f6e318cde2b80a72de40dab19eb7f76d3b6573a08e446bce6fb4435cdb016ae6489973b855a9bddd3b11/001</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>digits</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>AstorMain-digits-21</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>/Users/ruizhengu/Experiments/APR-as-AAT/IntroClassJava/dataset/digits/d5059e2b1493f91b32bb0c2c846d8461c50356f709a91792b6b625e112675de4edac2a09fa627d58c4651c662bbcf2c477660469b9327ed9427b43c25e4e070c/000</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>digits</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>AstorMain-digits-28</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>/Users/ruizhengu/Experiments/APR-as-AAT/IntroClassJava/dataset/digits/c5d8f924b86adfeafa7f520559aeb8bd0c3c178efe2500c4054c5ce51bcdbfc2da2e3d9fd5c73f559a7cb6c3b3555b04646111404744496cbcf31caa90e5beb4/003</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>digits</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>AstorMain-digits-54</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>/Users/ruizhengu/Experiments/APR-as-AAT/IntroClassJava/dataset/digits/0cdfa335eea3c612e6fa3ad261276b0c3ebbc6ff0ff13c20bdc249bad29a8037ca6dc887dd28558964e1e1a24f47c4cffc05adba525285dc8b93660cdf9b8b7c/006</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>digits</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>AstorMain-digits-56</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>/Users/ruizhengu/Experiments/APR-as-AAT/IntroClassJava/dataset/digits/0cdfa335eea3c612e6fa3ad261276b0c3ebbc6ff0ff13c20bdc249bad29a8037ca6dc887dd28558964e1e1a24f47c4cffc05adba525285dc8b93660cdf9b8b7c/005</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
add ref for grade
</commit_message>
<xml_diff>
--- a/repair-generation/results/results_introclass.xlsx
+++ b/repair-generation/results/results_introclass.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C38"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -453,221 +453,221 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>median</t>
+          <t>grade</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>AstorMain-median-2</t>
+          <t>AstorMain-grade-1</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>/Users/ruizhengu/Experiments/APR-as-AAT/IntroClassJava/dataset/median/fe9d5fb933c758c2cbbd859e3ecbd2d2eaecc2843b57cfd97da99af24de59f189a144d13ce81ec585d7c2f7367f70c0fb2aec8269eed1fd8380def614817ef7c/000</t>
+          <t>/Users/ruizhengu/Experiments/APR-as-AAT/IntroClassJava/dataset/grade/833bd42c11f7407d63f604b8ba3b7927e22e04e91884c959f01083cda7d5019610705b94a89c09cd1caa3fd1d58eee24b48b85b523db0fa3fc302e7af2dff93d/003</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>median</t>
+          <t>grade</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>AstorMain-median-3</t>
+          <t>AstorMain-grade-6</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>/Users/ruizhengu/Experiments/APR-as-AAT/IntroClassJava/dataset/median/fe9d5fb933c758c2cbbd859e3ecbd2d2eaecc2843b57cfd97da99af24de59f189a144d13ce81ec585d7c2f7367f70c0fb2aec8269eed1fd8380def614817ef7c/002</t>
+          <t>/Users/ruizhengu/Experiments/APR-as-AAT/IntroClassJava/dataset/grade/d8b262849e28496f80a8acf7de9758cf3f3a4edf023343521e2e0ac50ec485212a473405570d6c58de6756ae098600d9c7138390faa1aaf6bf3609a8d4016448/000</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>median</t>
+          <t>grade</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>AstorMain-median-12</t>
+          <t>AstorMain-grade-8</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>/Users/ruizhengu/Experiments/APR-as-AAT/IntroClassJava/dataset/median/48b82975576f07f162163145b334648a73321d003a0a8cd4577172e48ce4836e63953dffd4460a9a7aadc511a695ff93de0ce2baf953e4b78b747440caa736a6/000</t>
+          <t>/Users/ruizhengu/Experiments/APR-as-AAT/IntroClassJava/dataset/grade/769cd811312cbbb82c87033a78ac9584ad282550bcb9cc3ae8c4e3da44c288c1a5b3954e01998c3c0654ee6774ceab66e9fe5b135750905c917d2b0bb5fab98b/000</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>smallest</t>
+          <t>grade</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>AstorMain-smallest-4</t>
+          <t>AstorMain-grade-10</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>/Users/ruizhengu/Experiments/APR-as-AAT/IntroClassJava/dataset/smallest/88394fc00b7053b386e97564e28ef68421ae09c0baeaf887bba7e254f452419783ed8f774bff3c0c7d23bdc8f6c1443fb47c7af97323d4d3d63cc088d3b6841a/006</t>
+          <t>/Users/ruizhengu/Experiments/APR-as-AAT/IntroClassJava/dataset/grade/93f87bf20be12abd3b52e14015efb6d78b6038d2022e0ab5889979f9c6b6c8c757d6b5a59feae9f8415158057992ae837da76609dc156ea76b5cca7a43a4678b/015</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>smallest</t>
+          <t>grade</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>AstorMain-smallest-13</t>
+          <t>AstorMain-grade-20</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>/Users/ruizhengu/Experiments/APR-as-AAT/IntroClassJava/dataset/smallest/769cd811312cbbb82c87033a78ac9584ad282550bcb9cc3ae8c4e3da44c288c1a5b3954e01998c3c0654ee6774ceab66e9fe5b135750905c917d2b0bb5fab98b/003</t>
+          <t>/Users/ruizhengu/Experiments/APR-as-AAT/IntroClassJava/dataset/grade/1c2bb3a40a82cba97b2937bc6825903a28ecfe91f993fc177a0f2ae003bcc7b1073eb49e35d3f0f69d6b612e8347e9c1b93306bf25a7e5390098c1a06845baac/003</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>smallest</t>
+          <t>grade</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>AstorMain-smallest-15</t>
+          <t>AstorMain-grade-33</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>/Users/ruizhengu/Experiments/APR-as-AAT/IntroClassJava/dataset/smallest/769cd811312cbbb82c87033a78ac9584ad282550bcb9cc3ae8c4e3da44c288c1a5b3954e01998c3c0654ee6774ceab66e9fe5b135750905c917d2b0bb5fab98b/002</t>
+          <t>/Users/ruizhengu/Experiments/APR-as-AAT/IntroClassJava/dataset/grade/d6364e6e98a5c96387950d5b3e6206ba9d57628ab2ad0f2cd05ea7af3b818ed03e514157fe4c64e264a0ac9df0840028e0c5a8fd3d096f5ab93bffba61f23812/007</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>smallest</t>
+          <t>grade</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>AstorMain-smallest-27</t>
+          <t>AstorMain-grade-46</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>/Users/ruizhengu/Experiments/APR-as-AAT/IntroClassJava/dataset/smallest/3b2376ab97bb5d1a5dbbf2b45cf062db320757549c761936d19df05e856de894e45695014cd8063cdc22148b13fa1803b3c9e77356931d66f4fbec0efacf7829/008</t>
+          <t>/Users/ruizhengu/Experiments/APR-as-AAT/IntroClassJava/dataset/grade/e23b96b6bab26bd14316cefafcbaa16dd8eafcfb97a7159a7772f3c8bb3e78fb353dea728f6b4df6528286af5f0b85fd134c79886c9c2a352fe80d8204c69111/004</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>smallest</t>
+          <t>grade</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>AstorMain-smallest-28</t>
+          <t>AstorMain-grade-53</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>/Users/ruizhengu/Experiments/APR-as-AAT/IntroClassJava/dataset/smallest/3b2376ab97bb5d1a5dbbf2b45cf062db320757549c761936d19df05e856de894e45695014cd8063cdc22148b13fa1803b3c9e77356931d66f4fbec0efacf7829/006</t>
+          <t>/Users/ruizhengu/Experiments/APR-as-AAT/IntroClassJava/dataset/grade/98d873cde39437ae581e6b61ce30ca54634c9c1517b46a0f2774cb12db474b5a37759281b19283c60dbcfa44ac3e05d474a896310f64e8533603b1db73457494/004</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>smallest</t>
+          <t>grade</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>AstorMain-smallest-32</t>
+          <t>AstorMain-grade-55</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>/Users/ruizhengu/Experiments/APR-as-AAT/IntroClassJava/dataset/smallest/f8d57deac89e46f99354a70e8f6bc830e0bded0c297d7a0765348de79d6071cb076d4e8f2cd60cff584cb220049d6065827a29904a7e1f9144f510f7773e6d0e/000</t>
+          <t>/Users/ruizhengu/Experiments/APR-as-AAT/IntroClassJava/dataset/grade/f5b56c79c624eac7c37c45c1540916bb9b5f5db93e2a426a282a5d0eacde86b4b1e5d1d119eeb06f0ead94d2e4f228dca8dde4ef511af4bc59a18d272d820a0e/010</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>smallest</t>
+          <t>grade</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>AstorMain-smallest-35</t>
+          <t>AstorMain-grade-56</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>/Users/ruizhengu/Experiments/APR-as-AAT/IntroClassJava/dataset/smallest/dedc2a7c919835ade6d92729cfb18fc71addf6dcdf36ce26ca8b1e3d3aea81bad974c61b96fd71537e95a6aac4582d5b08f9fd8057ce40fb18fb5df37d86b70d/000</t>
+          <t>/Users/ruizhengu/Experiments/APR-as-AAT/IntroClassJava/dataset/grade/ee1f20ccded21df47f14019584a29968013d1e66c8df14c1564aff0d69f463c1897e93b7881fa6318cbf475b51e0cdd7523d748525fb5d64d376b88614d3fc92/000</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>smallest</t>
+          <t>grade</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>AstorMain-smallest-40</t>
+          <t>AstorMain-grade-58</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>/Users/ruizhengu/Experiments/APR-as-AAT/IntroClassJava/dataset/smallest/95362737dcd262ddd67b0fe1381c25f1e6b885860b4e51efb6f57223dceb77b4c6c7d855e3fe891c10cd51b48c9b052cf2c74f181a28d3020d77a4a2d6e4db18/009</t>
+          <t>/Users/ruizhengu/Experiments/APR-as-AAT/IntroClassJava/dataset/grade/489253253c866aa61b6b0d95c6072d3912f6b78dfbc01bdb2fbb663aefe33d6d353b1a61bb5fc567c9d6c334994111816edd3d43db47e4ea4a84953198736ff7/010</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>smallest</t>
+          <t>grade</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>AstorMain-smallest-46</t>
+          <t>AstorMain-grade-59</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>/Users/ruizhengu/Experiments/APR-as-AAT/IntroClassJava/dataset/smallest/36d8008b13f6475ca8fa4553fea10042b0a6c623665065672051445c3464d61b29b47cb66321844a0264505a0f5ccf5aa6de072aa266b5a8b0cf13198380a389/003</t>
+          <t>/Users/ruizhengu/Experiments/APR-as-AAT/IntroClassJava/dataset/grade/cd2d9b5b5cff96b07c5b22c0d139ffa2aa36b01823c9eb4db6eca19065a0ce2c4d2516bfcc2f1bc95daeae5b0bbd5e9c15b83feda776735e7bc3de6c49d25144/013</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>smallest</t>
+          <t>grade</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>AstorMain-smallest-48</t>
+          <t>AstorMain-grade-73</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>/Users/ruizhengu/Experiments/APR-as-AAT/IntroClassJava/dataset/smallest/97f6b15278788d90f6a0159ac65668f63f182fadf165e78bfecd7750de89f8611759f8d8206b3505407f7de14d124db7b0309a53e222c538c4dedadc6fa24fe6/003</t>
+          <t>/Users/ruizhengu/Experiments/APR-as-AAT/IntroClassJava/dataset/grade/0cea42f9680f35f5a84c724c396d4d588b65c303453f9585562f2e2af8db74f5096a83a70b17c5126538222b111a0795a34e9fb6db95d62d771d01592abe3ff6/003</t>
         </is>
       </c>
     </row>
@@ -679,12 +679,12 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>AstorMain-grade-1</t>
+          <t>AstorMain-grade-76</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>/Users/ruizhengu/Experiments/APR-as-AAT/IntroClassJava/dataset/grade/833bd42c11f7407d63f604b8ba3b7927e22e04e91884c959f01083cda7d5019610705b94a89c09cd1caa3fd1d58eee24b48b85b523db0fa3fc302e7af2dff93d/003</t>
+          <t>/Users/ruizhengu/Experiments/APR-as-AAT/IntroClassJava/dataset/grade/dccb1242e60245b164eba39e7c2ae4d7140c2c8964675ee78c7d8bea4aae494217dcac52415ab45fd89391060d17b101d87530b8e5a0b9a5781d06fe7db614eb/001</t>
         </is>
       </c>
     </row>
@@ -696,12 +696,12 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>AstorMain-grade-6</t>
+          <t>AstorMain-grade-77</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>/Users/ruizhengu/Experiments/APR-as-AAT/IntroClassJava/dataset/grade/d8b262849e28496f80a8acf7de9758cf3f3a4edf023343521e2e0ac50ec485212a473405570d6c58de6756ae098600d9c7138390faa1aaf6bf3609a8d4016448/000</t>
+          <t>/Users/ruizhengu/Experiments/APR-as-AAT/IntroClassJava/dataset/grade/5b504b3547416bfd54f138b3caa529ad72d157744b787e0e6f4745a2ff0fc5cc33bc87904b2d7cda9c7858087b2e04ece46d53fe9edd208f68d30a0ae70f363f/000</t>
         </is>
       </c>
     </row>
@@ -713,12 +713,12 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>AstorMain-grade-8</t>
+          <t>AstorMain-grade-79</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>/Users/ruizhengu/Experiments/APR-as-AAT/IntroClassJava/dataset/grade/769cd811312cbbb82c87033a78ac9584ad282550bcb9cc3ae8c4e3da44c288c1a5b3954e01998c3c0654ee6774ceab66e9fe5b135750905c917d2b0bb5fab98b/000</t>
+          <t>/Users/ruizhengu/Experiments/APR-as-AAT/IntroClassJava/dataset/grade/36d8008b13f6475ca8fa4553fea10042b0a6c623665065672051445c3464d61b29b47cb66321844a0264505a0f5ccf5aa6de072aa266b5a8b0cf13198380a389/000</t>
         </is>
       </c>
     </row>
@@ -730,352 +730,12 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>AstorMain-grade-10</t>
+          <t>AstorMain-grade-88</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>/Users/ruizhengu/Experiments/APR-as-AAT/IntroClassJava/dataset/grade/93f87bf20be12abd3b52e14015efb6d78b6038d2022e0ab5889979f9c6b6c8c757d6b5a59feae9f8415158057992ae837da76609dc156ea76b5cca7a43a4678b/015</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>grade</t>
-        </is>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>AstorMain-grade-20</t>
-        </is>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>/Users/ruizhengu/Experiments/APR-as-AAT/IntroClassJava/dataset/grade/1c2bb3a40a82cba97b2937bc6825903a28ecfe91f993fc177a0f2ae003bcc7b1073eb49e35d3f0f69d6b612e8347e9c1b93306bf25a7e5390098c1a06845baac/003</t>
-        </is>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>grade</t>
-        </is>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>AstorMain-grade-33</t>
-        </is>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>/Users/ruizhengu/Experiments/APR-as-AAT/IntroClassJava/dataset/grade/d6364e6e98a5c96387950d5b3e6206ba9d57628ab2ad0f2cd05ea7af3b818ed03e514157fe4c64e264a0ac9df0840028e0c5a8fd3d096f5ab93bffba61f23812/007</t>
-        </is>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>grade</t>
-        </is>
-      </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>AstorMain-grade-36</t>
-        </is>
-      </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>/Users/ruizhengu/Experiments/APR-as-AAT/IntroClassJava/dataset/grade/a0e3fdae706d528dcf146cbad986ba9fd834440a7b500e32f04fad073e955a46e481c713ee118432f3fd5dfa1a63fc1caefd648a56a389e40e6362dfd51625b0/012</t>
-        </is>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>grade</t>
-        </is>
-      </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>AstorMain-grade-37</t>
-        </is>
-      </c>
-      <c r="C22" t="inlineStr">
-        <is>
-          <t>/Users/ruizhengu/Experiments/APR-as-AAT/IntroClassJava/dataset/grade/a0e3fdae706d528dcf146cbad986ba9fd834440a7b500e32f04fad073e955a46e481c713ee118432f3fd5dfa1a63fc1caefd648a56a389e40e6362dfd51625b0/010</t>
-        </is>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>grade</t>
-        </is>
-      </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>AstorMain-grade-45</t>
-        </is>
-      </c>
-      <c r="C23" t="inlineStr">
-        <is>
-          <t>/Users/ruizhengu/Experiments/APR-as-AAT/IntroClassJava/dataset/grade/e23b96b6bab26bd14316cefafcbaa16dd8eafcfb97a7159a7772f3c8bb3e78fb353dea728f6b4df6528286af5f0b85fd134c79886c9c2a352fe80d8204c69111/003</t>
-        </is>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>grade</t>
-        </is>
-      </c>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>AstorMain-grade-46</t>
-        </is>
-      </c>
-      <c r="C24" t="inlineStr">
-        <is>
-          <t>/Users/ruizhengu/Experiments/APR-as-AAT/IntroClassJava/dataset/grade/e23b96b6bab26bd14316cefafcbaa16dd8eafcfb97a7159a7772f3c8bb3e78fb353dea728f6b4df6528286af5f0b85fd134c79886c9c2a352fe80d8204c69111/004</t>
-        </is>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="inlineStr">
-        <is>
-          <t>grade</t>
-        </is>
-      </c>
-      <c r="B25" t="inlineStr">
-        <is>
-          <t>AstorMain-grade-55</t>
-        </is>
-      </c>
-      <c r="C25" t="inlineStr">
-        <is>
-          <t>/Users/ruizhengu/Experiments/APR-as-AAT/IntroClassJava/dataset/grade/f5b56c79c624eac7c37c45c1540916bb9b5f5db93e2a426a282a5d0eacde86b4b1e5d1d119eeb06f0ead94d2e4f228dca8dde4ef511af4bc59a18d272d820a0e/010</t>
-        </is>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="inlineStr">
-        <is>
-          <t>grade</t>
-        </is>
-      </c>
-      <c r="B26" t="inlineStr">
-        <is>
-          <t>AstorMain-grade-56</t>
-        </is>
-      </c>
-      <c r="C26" t="inlineStr">
-        <is>
-          <t>/Users/ruizhengu/Experiments/APR-as-AAT/IntroClassJava/dataset/grade/ee1f20ccded21df47f14019584a29968013d1e66c8df14c1564aff0d69f463c1897e93b7881fa6318cbf475b51e0cdd7523d748525fb5d64d376b88614d3fc92/000</t>
-        </is>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="inlineStr">
-        <is>
-          <t>grade</t>
-        </is>
-      </c>
-      <c r="B27" t="inlineStr">
-        <is>
-          <t>AstorMain-grade-58</t>
-        </is>
-      </c>
-      <c r="C27" t="inlineStr">
-        <is>
-          <t>/Users/ruizhengu/Experiments/APR-as-AAT/IntroClassJava/dataset/grade/489253253c866aa61b6b0d95c6072d3912f6b78dfbc01bdb2fbb663aefe33d6d353b1a61bb5fc567c9d6c334994111816edd3d43db47e4ea4a84953198736ff7/010</t>
-        </is>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="inlineStr">
-        <is>
-          <t>grade</t>
-        </is>
-      </c>
-      <c r="B28" t="inlineStr">
-        <is>
-          <t>AstorMain-grade-59</t>
-        </is>
-      </c>
-      <c r="C28" t="inlineStr">
-        <is>
-          <t>/Users/ruizhengu/Experiments/APR-as-AAT/IntroClassJava/dataset/grade/cd2d9b5b5cff96b07c5b22c0d139ffa2aa36b01823c9eb4db6eca19065a0ce2c4d2516bfcc2f1bc95daeae5b0bbd5e9c15b83feda776735e7bc3de6c49d25144/013</t>
-        </is>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" t="inlineStr">
-        <is>
-          <t>grade</t>
-        </is>
-      </c>
-      <c r="B29" t="inlineStr">
-        <is>
-          <t>AstorMain-grade-76</t>
-        </is>
-      </c>
-      <c r="C29" t="inlineStr">
-        <is>
-          <t>/Users/ruizhengu/Experiments/APR-as-AAT/IntroClassJava/dataset/grade/dccb1242e60245b164eba39e7c2ae4d7140c2c8964675ee78c7d8bea4aae494217dcac52415ab45fd89391060d17b101d87530b8e5a0b9a5781d06fe7db614eb/001</t>
-        </is>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" t="inlineStr">
-        <is>
-          <t>grade</t>
-        </is>
-      </c>
-      <c r="B30" t="inlineStr">
-        <is>
-          <t>AstorMain-grade-77</t>
-        </is>
-      </c>
-      <c r="C30" t="inlineStr">
-        <is>
-          <t>/Users/ruizhengu/Experiments/APR-as-AAT/IntroClassJava/dataset/grade/5b504b3547416bfd54f138b3caa529ad72d157744b787e0e6f4745a2ff0fc5cc33bc87904b2d7cda9c7858087b2e04ece46d53fe9edd208f68d30a0ae70f363f/000</t>
-        </is>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" t="inlineStr">
-        <is>
-          <t>grade</t>
-        </is>
-      </c>
-      <c r="B31" t="inlineStr">
-        <is>
-          <t>AstorMain-grade-79</t>
-        </is>
-      </c>
-      <c r="C31" t="inlineStr">
-        <is>
-          <t>/Users/ruizhengu/Experiments/APR-as-AAT/IntroClassJava/dataset/grade/36d8008b13f6475ca8fa4553fea10042b0a6c623665065672051445c3464d61b29b47cb66321844a0264505a0f5ccf5aa6de072aa266b5a8b0cf13198380a389/000</t>
-        </is>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" t="inlineStr">
-        <is>
-          <t>grade</t>
-        </is>
-      </c>
-      <c r="B32" t="inlineStr">
-        <is>
-          <t>AstorMain-grade-80</t>
-        </is>
-      </c>
-      <c r="C32" t="inlineStr">
-        <is>
-          <t>/Users/ruizhengu/Experiments/APR-as-AAT/IntroClassJava/dataset/grade/9083480332b4a5e4274f3bf5ef8bd5d1bd75048c0c066e574c27a2de6d919d658efc519e8b6a230a074eb5f2957d5768f4dc981a8e926c3a72993bc448a017f7/013</t>
-        </is>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" t="inlineStr">
-        <is>
-          <t>grade</t>
-        </is>
-      </c>
-      <c r="B33" t="inlineStr">
-        <is>
-          <t>AstorMain-grade-82</t>
-        </is>
-      </c>
-      <c r="C33" t="inlineStr">
-        <is>
-          <t>/Users/ruizhengu/Experiments/APR-as-AAT/IntroClassJava/dataset/grade/9083480332b4a5e4274f3bf5ef8bd5d1bd75048c0c066e574c27a2de6d919d658efc519e8b6a230a074eb5f2957d5768f4dc981a8e926c3a72993bc448a017f7/010</t>
-        </is>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" t="inlineStr">
-        <is>
-          <t>grade</t>
-        </is>
-      </c>
-      <c r="B34" t="inlineStr">
-        <is>
-          <t>AstorMain-grade-88</t>
-        </is>
-      </c>
-      <c r="C34" t="inlineStr">
-        <is>
           <t>/Users/ruizhengu/Experiments/APR-as-AAT/IntroClassJava/dataset/grade/cb243bebea400595cc274d1246f3307c507ba6a0e891f6e318cde2b80a72de40dab19eb7f76d3b6573a08e446bce6fb4435cdb016ae6489973b855a9bddd3b11/001</t>
-        </is>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" t="inlineStr">
-        <is>
-          <t>digits</t>
-        </is>
-      </c>
-      <c r="B35" t="inlineStr">
-        <is>
-          <t>AstorMain-digits-21</t>
-        </is>
-      </c>
-      <c r="C35" t="inlineStr">
-        <is>
-          <t>/Users/ruizhengu/Experiments/APR-as-AAT/IntroClassJava/dataset/digits/d5059e2b1493f91b32bb0c2c846d8461c50356f709a91792b6b625e112675de4edac2a09fa627d58c4651c662bbcf2c477660469b9327ed9427b43c25e4e070c/000</t>
-        </is>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" t="inlineStr">
-        <is>
-          <t>digits</t>
-        </is>
-      </c>
-      <c r="B36" t="inlineStr">
-        <is>
-          <t>AstorMain-digits-28</t>
-        </is>
-      </c>
-      <c r="C36" t="inlineStr">
-        <is>
-          <t>/Users/ruizhengu/Experiments/APR-as-AAT/IntroClassJava/dataset/digits/c5d8f924b86adfeafa7f520559aeb8bd0c3c178efe2500c4054c5ce51bcdbfc2da2e3d9fd5c73f559a7cb6c3b3555b04646111404744496cbcf31caa90e5beb4/003</t>
-        </is>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" t="inlineStr">
-        <is>
-          <t>digits</t>
-        </is>
-      </c>
-      <c r="B37" t="inlineStr">
-        <is>
-          <t>AstorMain-digits-54</t>
-        </is>
-      </c>
-      <c r="C37" t="inlineStr">
-        <is>
-          <t>/Users/ruizhengu/Experiments/APR-as-AAT/IntroClassJava/dataset/digits/0cdfa335eea3c612e6fa3ad261276b0c3ebbc6ff0ff13c20bdc249bad29a8037ca6dc887dd28558964e1e1a24f47c4cffc05adba525285dc8b93660cdf9b8b7c/006</t>
-        </is>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" t="inlineStr">
-        <is>
-          <t>digits</t>
-        </is>
-      </c>
-      <c r="B38" t="inlineStr">
-        <is>
-          <t>AstorMain-digits-56</t>
-        </is>
-      </c>
-      <c r="C38" t="inlineStr">
-        <is>
-          <t>/Users/ruizhengu/Experiments/APR-as-AAT/IntroClassJava/dataset/digits/0cdfa335eea3c612e6fa3ad261276b0c3ebbc6ff0ff13c20bdc249bad29a8037ca6dc887dd28558964e1e1a24f47c4cffc05adba525285dc8b93660cdf9b8b7c/005</t>
         </is>
       </c>
     </row>

</xml_diff>